<commit_message>
[excel-pipeline] hash_id:182be8a commit_msg:增加字段 ...
</commit_message>
<xml_diff>
--- a/config/excel/SkillBase.xlsx
+++ b/config/excel/SkillBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120859DA-DB5F-4738-AE77-E663D34C0831}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1BB2B3-243D-4767-BEC6-E02EF395ECA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillBase" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>dd</author>
   </authors>
   <commentList>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{D0F2A3A5-137E-4A82-8578-1041C1C6BD28}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{D0F2A3A5-137E-4A82-8578-1041C1C6BD28}">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
   <si>
     <t>行列头两行不会被读取</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -315,12 +315,6 @@
   <si>
     <t>多个技能效果
 数组格式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>以自身
-为圆心
-距离米</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -540,6 +534,62 @@
   <si>
     <t>进入战斗后，首次可使用该技能的冷却CD
 (秒)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出手范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>距离目标多远使用技能
+近战&lt;目标长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹道速度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否弹道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否是弹道的类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>插槽ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认是0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用模型上
+的插槽ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弹道初始位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命中消息点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被击动作编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>命中的时间点数组
+[]number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与命中数量相同，被击动作编号
+[]string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -724,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -783,11 +833,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="36">
     <dxf>
       <font>
         <b val="0"/>
@@ -1324,6 +1377,228 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -1875,19 +2150,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0F9482FB-F1A4-4850-86F8-C15BFC778075}" name="表5" displayName="表5" ref="C1:AC34" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="C1:AC34" xr:uid="{ACA1193D-CE65-4771-A649-26B6E9EA140E}"/>
-  <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{0E0EE31E-4EF4-47A6-A02C-B14555F7469B}" name="技能ID" dataDxfId="26"/>
-    <tableColumn id="22" xr3:uid="{E1A1EC3B-7958-4D16-B93D-47A83EFFF24F}" name="技能等级" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{F6C3B926-A1B3-4A1C-86C0-13E1D171263F}" name="技能名称" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{BF6A1109-3BD4-42E4-93C8-E96877E4684F}" name="技能描述" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{AD42AAEB-FC8C-4032-8705-5FFB55906D3C}" name="技能图标" dataDxfId="22"/>
-    <tableColumn id="25" xr3:uid="{5EB1F39C-170E-4500-9A1D-EA5FD9D84A16}" name="ACT条动作" dataDxfId="21"/>
-    <tableColumn id="20" xr3:uid="{DF235172-D925-4D3E-866F-35EB36B0A7E1}" name="前摇动作" dataDxfId="20"/>
-    <tableColumn id="26" xr3:uid="{33BA7F53-F2D3-4204-BC87-5E499710AF16}" name="技能动作" dataDxfId="19"/>
-    <tableColumn id="27" xr3:uid="{7B7E6045-E4B4-4249-843F-8B2096C39B45}" name="后摇动作" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{E8E90E8F-1995-4C61-A68C-8B81AC41A07E}" name="技能动画" dataDxfId="17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0F9482FB-F1A4-4850-86F8-C15BFC778075}" name="表5" displayName="表5" ref="C1:AI34" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+  <autoFilter ref="C1:AI34" xr:uid="{ACA1193D-CE65-4771-A649-26B6E9EA140E}"/>
+  <tableColumns count="33">
+    <tableColumn id="1" xr3:uid="{0E0EE31E-4EF4-47A6-A02C-B14555F7469B}" name="技能ID" dataDxfId="32"/>
+    <tableColumn id="22" xr3:uid="{E1A1EC3B-7958-4D16-B93D-47A83EFFF24F}" name="技能等级" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{F6C3B926-A1B3-4A1C-86C0-13E1D171263F}" name="技能名称" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{BF6A1109-3BD4-42E4-93C8-E96877E4684F}" name="技能描述" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{AD42AAEB-FC8C-4032-8705-5FFB55906D3C}" name="技能图标" dataDxfId="28"/>
+    <tableColumn id="25" xr3:uid="{5EB1F39C-170E-4500-9A1D-EA5FD9D84A16}" name="ACT条动作" dataDxfId="27"/>
+    <tableColumn id="20" xr3:uid="{DF235172-D925-4D3E-866F-35EB36B0A7E1}" name="前摇动作" dataDxfId="26"/>
+    <tableColumn id="26" xr3:uid="{33BA7F53-F2D3-4204-BC87-5E499710AF16}" name="技能动作" dataDxfId="25"/>
+    <tableColumn id="33" xr3:uid="{6E7D3F46-4A3D-4D38-B359-FE07A4079767}" name="命中消息点" dataDxfId="24"/>
+    <tableColumn id="32" xr3:uid="{38F5469B-B50A-447A-94E2-227AAA95BA4B}" name="被击动作编号" dataDxfId="23"/>
+    <tableColumn id="27" xr3:uid="{7B7E6045-E4B4-4249-843F-8B2096C39B45}" name="后摇动作" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{E8E90E8F-1995-4C61-A68C-8B81AC41A07E}" name="技能动画" dataDxfId="21"/>
+    <tableColumn id="31" xr3:uid="{5A9F6830-8322-4EB4-A36B-D92752656B11}" name="弹道初始位置" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{3F5FA866-1408-4A54-848B-79617FC1D727}" name="插槽ID" dataDxfId="19"/>
+    <tableColumn id="29" xr3:uid="{3D757DC9-E31E-4011-9972-17FCD11CA685}" name="是否弹道" dataDxfId="18"/>
+    <tableColumn id="30" xr3:uid="{9D219D1E-C382-4CBB-A03F-A5A973C866AF}" name="弹道速度" dataDxfId="17"/>
     <tableColumn id="6" xr3:uid="{3ABDB000-A48D-43AE-B45C-97BDD2171745}" name="技能类型" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{A2C44567-4D04-448D-B510-5BBC9CEFB2D9}" name="ACT条速度" dataDxfId="15"/>
     <tableColumn id="28" xr3:uid="{7B7EE486-2B33-46A4-850E-FE81E686F065}" name="ACT秒" dataDxfId="14">
@@ -1898,7 +2179,7 @@
     <tableColumn id="10" xr3:uid="{CDDA707B-D347-4FF6-87DA-424E0D935A3E}" name="初始CD" dataDxfId="11"/>
     <tableColumn id="11" xr3:uid="{BAC0605C-4D75-47A9-966F-F88AE32FC0D8}" name="回转CD" dataDxfId="10"/>
     <tableColumn id="12" xr3:uid="{1B5EF81A-42C1-4ABA-9344-C6A99BE25752}" name="次数限制" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{56EA1AC2-2D75-4ECA-AD42-6DEB09A89621}" name="施法范围" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{56EA1AC2-2D75-4ECA-AD42-6DEB09A89621}" name="出手范围" dataDxfId="8"/>
     <tableColumn id="14" xr3:uid="{BA72201D-9EED-4B06-A696-7CF31B0A111F}" name="主目标_x000a_范围类型" dataDxfId="7"/>
     <tableColumn id="15" xr3:uid="{A1D82393-11AC-4336-BF23-F777E5F410C1}" name="主目标类型" dataDxfId="6"/>
     <tableColumn id="16" xr3:uid="{029C5084-1ADB-4FF0-9EBA-349BC28A742D}" name="目标范围长" dataDxfId="5"/>
@@ -2175,24 +2456,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC34"/>
+  <dimension ref="A1:AI34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="13" width="10.625" style="1"/>
-    <col min="14" max="16" width="11.75" style="1" customWidth="1"/>
-    <col min="17" max="22" width="10.625" style="1"/>
-    <col min="23" max="25" width="12.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.625" style="1"/>
+    <col min="1" max="18" width="10.625" style="1"/>
+    <col min="20" max="20" width="10.625" style="1"/>
+    <col min="21" max="23" width="11.75" style="1" customWidth="1"/>
+    <col min="24" max="29" width="10.625" style="1"/>
+    <col min="30" max="32" width="12.125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2203,7 +2485,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>5</v>
@@ -2215,81 +2497,99 @@
         <v>15</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J1" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="O1" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="T1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="P1" s="15" t="s">
+      <c r="U1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="V1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="AD1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="AE1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AH1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AC1" s="18" t="s">
-        <v>71</v>
-      </c>
     </row>
-    <row r="2" spans="1:29" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>51</v>
@@ -2299,71 +2599,87 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="T2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="U2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="W2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH2" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="19" t="s">
+      <c r="AI2" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="AC2" s="19" t="s">
-        <v>97</v>
-      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2371,7 +2687,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>8</v>
@@ -2383,67 +2699,73 @@
         <v>14</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7" t="s">
+      <c r="U3" s="7"/>
+      <c r="V3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="W3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="AA3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="AB3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="AC3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="AD3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="AE3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="AF3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AG3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2451,7 +2773,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>6</v>
@@ -2463,69 +2785,75 @@
         <v>13</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="L4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7" t="s">
+      <c r="T4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="W4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="X4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="Y4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="Z4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="AA4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="7" t="s">
+      <c r="AB4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="AC4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="AD4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="Y4" s="7" t="s">
+      <c r="AE4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="AF4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="7" t="s">
+      <c r="AG4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -2554,8 +2882,14 @@
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2575,56 +2909,44 @@
         <v>23</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="T6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>100</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="U6" s="7"/>
       <c r="V6" s="7" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z6" s="7" t="s">
         <v>9</v>
@@ -2632,10 +2954,28 @@
       <c r="AA6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
+      <c r="AB6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C7" s="12">
         <v>101001</v>
       </c>
@@ -2650,56 +2990,62 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
-      <c r="N7" s="6">
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6">
+        <v>1</v>
+      </c>
+      <c r="T7" s="6">
         <v>0.5</v>
       </c>
-      <c r="O7" s="6">
+      <c r="U7" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>2</v>
       </c>
-      <c r="P7" s="6">
+      <c r="V7" s="6">
         <v>10</v>
       </c>
-      <c r="Q7" s="6">
-        <v>0</v>
-      </c>
-      <c r="R7" s="6">
-        <v>0</v>
-      </c>
-      <c r="S7" s="6">
-        <v>0</v>
-      </c>
-      <c r="T7" s="6">
-        <v>1</v>
-      </c>
-      <c r="U7" s="6">
+      <c r="W7" s="6">
+        <v>0</v>
+      </c>
+      <c r="X7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="6">
         <v>2</v>
       </c>
-      <c r="V7" s="6">
-        <v>1</v>
-      </c>
-      <c r="W7" s="6">
-        <v>4</v>
-      </c>
-      <c r="X7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="6">
+      <c r="AB7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="6">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>2</v>
+      </c>
+      <c r="AE7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C8" s="13">
         <v>101002</v>
       </c>
@@ -2714,56 +3060,62 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="8">
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8">
         <v>2</v>
       </c>
-      <c r="N8" s="8">
-        <v>1</v>
-      </c>
-      <c r="O8" s="6">
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
+      <c r="U8" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>1</v>
       </c>
-      <c r="P8" s="8">
+      <c r="V8" s="8">
         <v>20</v>
       </c>
-      <c r="Q8" s="8">
-        <v>0</v>
-      </c>
-      <c r="R8" s="8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="8">
-        <v>1</v>
-      </c>
-      <c r="T8" s="8">
-        <v>1</v>
-      </c>
-      <c r="U8" s="8">
+      <c r="W8" s="8">
+        <v>0</v>
+      </c>
+      <c r="X8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="8">
         <v>10</v>
       </c>
-      <c r="V8" s="8">
-        <v>1</v>
-      </c>
-      <c r="W8" s="8">
-        <v>4</v>
-      </c>
-      <c r="X8" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y8" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="8">
+      <c r="AB8" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD8" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="8">
         <v>5</v>
       </c>
-      <c r="AA8" s="8">
+      <c r="AG8" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C9" s="12">
         <v>101003</v>
       </c>
@@ -2778,56 +3130,62 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6">
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6">
         <v>3</v>
       </c>
-      <c r="N9" s="6">
+      <c r="T9" s="6">
         <v>2</v>
       </c>
-      <c r="O9" s="6">
+      <c r="U9" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>0.5</v>
       </c>
-      <c r="P9" s="6">
+      <c r="V9" s="6">
         <v>-100</v>
       </c>
-      <c r="Q9" s="6">
-        <v>0</v>
-      </c>
-      <c r="R9" s="6">
-        <v>0</v>
-      </c>
-      <c r="S9" s="6">
+      <c r="W9" s="6">
+        <v>0</v>
+      </c>
+      <c r="X9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="6">
         <v>2</v>
       </c>
-      <c r="T9" s="6">
-        <v>1</v>
-      </c>
-      <c r="U9" s="6">
+      <c r="Z9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="6">
         <v>40</v>
       </c>
-      <c r="V9" s="6">
-        <v>1</v>
-      </c>
-      <c r="W9" s="6">
-        <v>4</v>
-      </c>
-      <c r="X9" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="6">
+      <c r="AB9" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>4</v>
+      </c>
+      <c r="AE9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="6">
         <v>5</v>
       </c>
-      <c r="AA9" s="6">
+      <c r="AG9" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C10" s="13">
         <v>101004</v>
       </c>
@@ -2842,56 +3200,62 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="8">
-        <v>4</v>
-      </c>
-      <c r="N10" s="8">
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8">
+        <v>4</v>
+      </c>
+      <c r="T10" s="8">
         <v>0.2</v>
       </c>
-      <c r="O10" s="6">
+      <c r="U10" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>5</v>
       </c>
-      <c r="P10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="8">
+      <c r="V10" s="8">
+        <v>0</v>
+      </c>
+      <c r="W10" s="8">
         <v>20</v>
       </c>
-      <c r="R10" s="8">
-        <v>0</v>
-      </c>
-      <c r="S10" s="8">
+      <c r="X10" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="8">
         <v>1.5</v>
       </c>
-      <c r="T10" s="8">
-        <v>1</v>
-      </c>
-      <c r="U10" s="8">
+      <c r="Z10" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="8">
         <v>20</v>
       </c>
-      <c r="V10" s="8">
-        <v>1</v>
-      </c>
-      <c r="W10" s="8">
-        <v>4</v>
-      </c>
-      <c r="X10" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="8">
+      <c r="AB10" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="8">
         <v>5</v>
       </c>
-      <c r="AA10" s="8">
+      <c r="AG10" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C11" s="12">
         <v>102001</v>
       </c>
@@ -2906,39 +3270,27 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6">
+        <v>1</v>
+      </c>
+      <c r="T11" s="6">
         <v>0.5</v>
       </c>
-      <c r="O11" s="6">
+      <c r="U11" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>2</v>
       </c>
-      <c r="P11" s="6">
+      <c r="V11" s="6">
         <v>10</v>
       </c>
-      <c r="Q11" s="6">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6">
-        <v>0</v>
-      </c>
-      <c r="T11" s="6">
-        <v>1</v>
-      </c>
-      <c r="U11" s="6">
-        <v>4</v>
-      </c>
-      <c r="V11" s="6">
-        <v>1</v>
-      </c>
       <c r="W11" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="X11" s="6">
         <v>0</v>
@@ -2950,12 +3302,30 @@
         <v>1</v>
       </c>
       <c r="AA11" s="6">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C12" s="13">
         <v>102002</v>
       </c>
@@ -2970,56 +3340,62 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="8">
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8">
         <v>2</v>
       </c>
-      <c r="N12" s="8">
-        <v>1</v>
-      </c>
-      <c r="O12" s="6">
+      <c r="T12" s="8">
+        <v>1</v>
+      </c>
+      <c r="U12" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>1</v>
       </c>
-      <c r="P12" s="8">
+      <c r="V12" s="8">
         <v>20</v>
       </c>
-      <c r="Q12" s="8">
-        <v>0</v>
-      </c>
-      <c r="R12" s="8">
-        <v>0</v>
-      </c>
-      <c r="S12" s="8">
-        <v>1</v>
-      </c>
-      <c r="T12" s="8">
-        <v>1</v>
-      </c>
-      <c r="U12" s="8">
+      <c r="W12" s="8">
+        <v>0</v>
+      </c>
+      <c r="X12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="8">
         <v>10</v>
       </c>
-      <c r="V12" s="8">
-        <v>1</v>
-      </c>
-      <c r="W12" s="8">
-        <v>4</v>
-      </c>
-      <c r="X12" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y12" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="8">
+      <c r="AB12" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD12" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="8">
         <v>5</v>
       </c>
-      <c r="AA12" s="8">
+      <c r="AG12" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C13" s="12">
         <v>102003</v>
       </c>
@@ -3034,56 +3410,62 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="6">
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6">
         <v>3</v>
       </c>
-      <c r="N13" s="6">
+      <c r="T13" s="6">
         <v>2</v>
       </c>
-      <c r="O13" s="6">
+      <c r="U13" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>0.5</v>
       </c>
-      <c r="P13" s="6">
+      <c r="V13" s="6">
         <v>-100</v>
       </c>
-      <c r="Q13" s="6">
-        <v>0</v>
-      </c>
-      <c r="R13" s="6">
-        <v>0</v>
-      </c>
-      <c r="S13" s="6">
+      <c r="W13" s="6">
+        <v>0</v>
+      </c>
+      <c r="X13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="6">
         <v>2</v>
       </c>
-      <c r="T13" s="6">
-        <v>1</v>
-      </c>
-      <c r="U13" s="6">
+      <c r="Z13" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="6">
         <v>40</v>
       </c>
-      <c r="V13" s="6">
-        <v>1</v>
-      </c>
-      <c r="W13" s="6">
-        <v>4</v>
-      </c>
-      <c r="X13" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="6">
+      <c r="AB13" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="6">
+        <v>4</v>
+      </c>
+      <c r="AE13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="6">
         <v>5</v>
       </c>
-      <c r="AA13" s="6">
+      <c r="AG13" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C14" s="13">
         <v>102004</v>
       </c>
@@ -3098,56 +3480,62 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="8">
-        <v>4</v>
-      </c>
-      <c r="N14" s="8">
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8">
+        <v>4</v>
+      </c>
+      <c r="T14" s="8">
         <v>0.2</v>
       </c>
-      <c r="O14" s="6">
+      <c r="U14" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>5</v>
       </c>
-      <c r="P14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="8">
+      <c r="V14" s="8">
+        <v>0</v>
+      </c>
+      <c r="W14" s="8">
         <v>20</v>
       </c>
-      <c r="R14" s="8">
-        <v>0</v>
-      </c>
-      <c r="S14" s="8">
+      <c r="X14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="8">
         <v>1.5</v>
       </c>
-      <c r="T14" s="8">
-        <v>1</v>
-      </c>
-      <c r="U14" s="8">
+      <c r="Z14" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="8">
         <v>20</v>
       </c>
-      <c r="V14" s="8">
-        <v>1</v>
-      </c>
-      <c r="W14" s="8">
-        <v>4</v>
-      </c>
-      <c r="X14" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="8">
+      <c r="AB14" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD14" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="8">
         <v>5</v>
       </c>
-      <c r="AA14" s="8">
+      <c r="AG14" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C15" s="12">
         <v>103001</v>
       </c>
@@ -3162,56 +3550,62 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="6">
-        <v>1</v>
-      </c>
-      <c r="N15" s="6">
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6">
+        <v>1</v>
+      </c>
+      <c r="T15" s="6">
         <v>0.5</v>
       </c>
-      <c r="O15" s="6">
+      <c r="U15" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>2</v>
       </c>
-      <c r="P15" s="6">
+      <c r="V15" s="6">
         <v>10</v>
       </c>
-      <c r="Q15" s="6">
-        <v>0</v>
-      </c>
-      <c r="R15" s="6">
-        <v>0</v>
-      </c>
-      <c r="S15" s="6">
-        <v>0</v>
-      </c>
-      <c r="T15" s="6">
-        <v>1</v>
-      </c>
-      <c r="U15" s="6">
+      <c r="W15" s="6">
+        <v>0</v>
+      </c>
+      <c r="X15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="6">
         <v>12</v>
       </c>
-      <c r="V15" s="6">
-        <v>1</v>
-      </c>
-      <c r="W15" s="6">
-        <v>4</v>
-      </c>
-      <c r="X15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="6">
+      <c r="AB15" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C16" s="13">
         <v>103002</v>
       </c>
@@ -3226,56 +3620,62 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="8">
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8">
         <v>2</v>
       </c>
-      <c r="N16" s="8">
-        <v>1</v>
-      </c>
-      <c r="O16" s="6">
+      <c r="T16" s="8">
+        <v>1</v>
+      </c>
+      <c r="U16" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>1</v>
       </c>
-      <c r="P16" s="8">
+      <c r="V16" s="8">
         <v>20</v>
       </c>
-      <c r="Q16" s="8">
-        <v>0</v>
-      </c>
-      <c r="R16" s="8">
-        <v>0</v>
-      </c>
-      <c r="S16" s="8">
-        <v>1</v>
-      </c>
-      <c r="T16" s="8">
-        <v>1</v>
-      </c>
-      <c r="U16" s="8">
+      <c r="W16" s="8">
+        <v>0</v>
+      </c>
+      <c r="X16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="8">
         <v>16</v>
       </c>
-      <c r="V16" s="8">
-        <v>1</v>
-      </c>
-      <c r="W16" s="8">
-        <v>4</v>
-      </c>
-      <c r="X16" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y16" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="8">
+      <c r="AB16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD16" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="8">
         <v>5</v>
       </c>
-      <c r="AA16" s="8">
+      <c r="AG16" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
     </row>
-    <row r="17" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C17" s="12">
         <v>103003</v>
       </c>
@@ -3290,56 +3690,62 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="6">
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6">
         <v>3</v>
       </c>
-      <c r="N17" s="6">
+      <c r="T17" s="6">
         <v>2</v>
       </c>
-      <c r="O17" s="6">
+      <c r="U17" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>0.5</v>
       </c>
-      <c r="P17" s="6">
+      <c r="V17" s="6">
         <v>-100</v>
       </c>
-      <c r="Q17" s="6">
-        <v>0</v>
-      </c>
-      <c r="R17" s="6">
-        <v>0</v>
-      </c>
-      <c r="S17" s="6">
+      <c r="W17" s="6">
+        <v>0</v>
+      </c>
+      <c r="X17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="6">
         <v>2</v>
       </c>
-      <c r="T17" s="6">
-        <v>1</v>
-      </c>
-      <c r="U17" s="6">
+      <c r="Z17" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="6">
         <v>40</v>
       </c>
-      <c r="V17" s="6">
-        <v>1</v>
-      </c>
-      <c r="W17" s="6">
-        <v>4</v>
-      </c>
-      <c r="X17" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y17" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="6">
+      <c r="AB17" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="6">
+        <v>4</v>
+      </c>
+      <c r="AE17" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="6">
         <v>5</v>
       </c>
-      <c r="AA17" s="6">
+      <c r="AG17" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
     </row>
-    <row r="18" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C18" s="13">
         <v>103004</v>
       </c>
@@ -3354,56 +3760,62 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="8">
-        <v>4</v>
-      </c>
-      <c r="N18" s="8">
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8">
+        <v>4</v>
+      </c>
+      <c r="T18" s="8">
         <v>0.2</v>
       </c>
-      <c r="O18" s="6">
+      <c r="U18" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>5</v>
       </c>
-      <c r="P18" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="8">
+      <c r="V18" s="8">
+        <v>0</v>
+      </c>
+      <c r="W18" s="8">
         <v>20</v>
       </c>
-      <c r="R18" s="8">
-        <v>0</v>
-      </c>
-      <c r="S18" s="8">
+      <c r="X18" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="8">
         <v>1.5</v>
       </c>
-      <c r="T18" s="8">
-        <v>1</v>
-      </c>
-      <c r="U18" s="8">
+      <c r="Z18" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="8">
         <v>20</v>
       </c>
-      <c r="V18" s="8">
-        <v>1</v>
-      </c>
-      <c r="W18" s="8">
-        <v>4</v>
-      </c>
-      <c r="X18" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y18" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="8">
+      <c r="AB18" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD18" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE18" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="8">
         <v>5</v>
       </c>
-      <c r="AA18" s="8">
+      <c r="AG18" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB18" s="8"/>
-      <c r="AC18" s="8"/>
+      <c r="AH18" s="8"/>
+      <c r="AI18" s="8"/>
     </row>
-    <row r="19" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C19" s="12">
         <v>104001</v>
       </c>
@@ -3418,56 +3830,62 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="6">
-        <v>1</v>
-      </c>
-      <c r="N19" s="6">
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6">
+        <v>1</v>
+      </c>
+      <c r="T19" s="6">
         <v>0.5</v>
       </c>
-      <c r="O19" s="6">
+      <c r="U19" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>2</v>
       </c>
-      <c r="P19" s="6">
+      <c r="V19" s="6">
         <v>10</v>
       </c>
-      <c r="Q19" s="6">
-        <v>0</v>
-      </c>
-      <c r="R19" s="6">
-        <v>0</v>
-      </c>
-      <c r="S19" s="6">
-        <v>0</v>
-      </c>
-      <c r="T19" s="6">
-        <v>1</v>
-      </c>
-      <c r="U19" s="6">
+      <c r="W19" s="6">
+        <v>0</v>
+      </c>
+      <c r="X19" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="6">
         <v>12</v>
       </c>
-      <c r="V19" s="6">
-        <v>1</v>
-      </c>
-      <c r="W19" s="6">
-        <v>4</v>
-      </c>
-      <c r="X19" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="6">
+      <c r="AB19" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD19" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AI19" s="6"/>
     </row>
-    <row r="20" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C20" s="13">
         <v>104002</v>
       </c>
@@ -3482,56 +3900,62 @@
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="8">
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8">
         <v>2</v>
       </c>
-      <c r="N20" s="8">
-        <v>1</v>
-      </c>
-      <c r="O20" s="6">
+      <c r="T20" s="8">
+        <v>1</v>
+      </c>
+      <c r="U20" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>1</v>
       </c>
-      <c r="P20" s="8">
+      <c r="V20" s="8">
         <v>20</v>
       </c>
-      <c r="Q20" s="8">
-        <v>0</v>
-      </c>
-      <c r="R20" s="8">
-        <v>0</v>
-      </c>
-      <c r="S20" s="8">
-        <v>1</v>
-      </c>
-      <c r="T20" s="8">
-        <v>1</v>
-      </c>
-      <c r="U20" s="8">
+      <c r="W20" s="8">
+        <v>0</v>
+      </c>
+      <c r="X20" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="8">
         <v>16</v>
       </c>
-      <c r="V20" s="8">
-        <v>1</v>
-      </c>
-      <c r="W20" s="8">
-        <v>4</v>
-      </c>
-      <c r="X20" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y20" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="8">
+      <c r="AB20" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD20" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE20" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="8">
         <v>5</v>
       </c>
-      <c r="AA20" s="8">
+      <c r="AG20" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB20" s="8"/>
-      <c r="AC20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
     </row>
-    <row r="21" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C21" s="12">
         <v>104003</v>
       </c>
@@ -3546,56 +3970,62 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-      <c r="M21" s="6">
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6">
         <v>3</v>
       </c>
-      <c r="N21" s="6">
+      <c r="T21" s="6">
         <v>2</v>
       </c>
-      <c r="O21" s="6">
+      <c r="U21" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>0.5</v>
       </c>
-      <c r="P21" s="6">
+      <c r="V21" s="6">
         <v>-100</v>
       </c>
-      <c r="Q21" s="6">
-        <v>0</v>
-      </c>
-      <c r="R21" s="6">
-        <v>0</v>
-      </c>
-      <c r="S21" s="6">
+      <c r="W21" s="6">
+        <v>0</v>
+      </c>
+      <c r="X21" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="6">
         <v>2</v>
       </c>
-      <c r="T21" s="6">
-        <v>1</v>
-      </c>
-      <c r="U21" s="6">
+      <c r="Z21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="6">
         <v>40</v>
       </c>
-      <c r="V21" s="6">
-        <v>1</v>
-      </c>
-      <c r="W21" s="6">
-        <v>4</v>
-      </c>
-      <c r="X21" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y21" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="6">
+      <c r="AB21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD21" s="6">
+        <v>4</v>
+      </c>
+      <c r="AE21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="6">
         <v>5</v>
       </c>
-      <c r="AA21" s="6">
+      <c r="AG21" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB21" s="6"/>
-      <c r="AC21" s="6"/>
+      <c r="AH21" s="6"/>
+      <c r="AI21" s="6"/>
     </row>
-    <row r="22" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C22" s="13">
         <v>104004</v>
       </c>
@@ -3610,56 +4040,62 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="8">
-        <v>4</v>
-      </c>
-      <c r="N22" s="8">
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8">
+        <v>4</v>
+      </c>
+      <c r="T22" s="8">
         <v>0.2</v>
       </c>
-      <c r="O22" s="6">
+      <c r="U22" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>5</v>
       </c>
-      <c r="P22" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="8">
+      <c r="V22" s="8">
+        <v>0</v>
+      </c>
+      <c r="W22" s="8">
         <v>20</v>
       </c>
-      <c r="R22" s="8">
-        <v>0</v>
-      </c>
-      <c r="S22" s="8">
+      <c r="X22" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="8">
         <v>1.5</v>
       </c>
-      <c r="T22" s="8">
-        <v>1</v>
-      </c>
-      <c r="U22" s="8">
+      <c r="Z22" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="8">
         <v>20</v>
       </c>
-      <c r="V22" s="8">
-        <v>1</v>
-      </c>
-      <c r="W22" s="8">
-        <v>4</v>
-      </c>
-      <c r="X22" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y22" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="8">
+      <c r="AB22" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD22" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE22" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="8">
         <v>5</v>
       </c>
-      <c r="AA22" s="8">
+      <c r="AG22" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB22" s="8"/>
-      <c r="AC22" s="8"/>
+      <c r="AH22" s="8"/>
+      <c r="AI22" s="8"/>
     </row>
-    <row r="23" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C23" s="12">
         <v>105001</v>
       </c>
@@ -3674,56 +4110,62 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="6">
-        <v>1</v>
-      </c>
-      <c r="N23" s="6">
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6">
+        <v>1</v>
+      </c>
+      <c r="T23" s="6">
         <v>0.5</v>
       </c>
-      <c r="O23" s="6">
+      <c r="U23" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>2</v>
       </c>
-      <c r="P23" s="6">
+      <c r="V23" s="6">
         <v>10</v>
       </c>
-      <c r="Q23" s="6">
-        <v>0</v>
-      </c>
-      <c r="R23" s="6">
-        <v>0</v>
-      </c>
-      <c r="S23" s="6">
-        <v>0</v>
-      </c>
-      <c r="T23" s="6">
-        <v>1</v>
-      </c>
-      <c r="U23" s="6">
+      <c r="W23" s="6">
+        <v>0</v>
+      </c>
+      <c r="X23" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="6">
         <v>2</v>
       </c>
-      <c r="V23" s="6">
-        <v>1</v>
-      </c>
-      <c r="W23" s="6">
-        <v>4</v>
-      </c>
-      <c r="X23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="6">
+      <c r="AB23" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC23" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD23" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
+      <c r="AH23" s="6"/>
+      <c r="AI23" s="6"/>
     </row>
-    <row r="24" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C24" s="13">
         <v>105002</v>
       </c>
@@ -3738,56 +4180,62 @@
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
-      <c r="M24" s="8">
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8">
         <v>2</v>
       </c>
-      <c r="N24" s="8">
-        <v>1</v>
-      </c>
-      <c r="O24" s="8">
+      <c r="T24" s="8">
+        <v>1</v>
+      </c>
+      <c r="U24" s="8">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>1</v>
       </c>
-      <c r="P24" s="8">
+      <c r="V24" s="8">
         <v>20</v>
       </c>
-      <c r="Q24" s="8">
-        <v>0</v>
-      </c>
-      <c r="R24" s="8">
-        <v>0</v>
-      </c>
-      <c r="S24" s="8">
-        <v>1</v>
-      </c>
-      <c r="T24" s="8">
-        <v>1</v>
-      </c>
-      <c r="U24" s="8">
+      <c r="W24" s="8">
+        <v>0</v>
+      </c>
+      <c r="X24" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="8">
         <v>10</v>
       </c>
-      <c r="V24" s="8">
-        <v>1</v>
-      </c>
-      <c r="W24" s="8">
-        <v>4</v>
-      </c>
-      <c r="X24" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y24" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="8">
+      <c r="AB24" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD24" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE24" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="8">
         <v>5</v>
       </c>
-      <c r="AA24" s="8">
+      <c r="AG24" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB24" s="8"/>
-      <c r="AC24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
     </row>
-    <row r="25" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C25" s="12">
         <v>105003</v>
       </c>
@@ -3802,56 +4250,62 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="6">
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6">
         <v>3</v>
       </c>
-      <c r="N25" s="6">
+      <c r="T25" s="6">
         <v>2</v>
       </c>
-      <c r="O25" s="6">
+      <c r="U25" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>0.5</v>
       </c>
-      <c r="P25" s="6">
+      <c r="V25" s="6">
         <v>-100</v>
       </c>
-      <c r="Q25" s="6">
-        <v>0</v>
-      </c>
-      <c r="R25" s="6">
-        <v>0</v>
-      </c>
-      <c r="S25" s="6">
+      <c r="W25" s="6">
+        <v>0</v>
+      </c>
+      <c r="X25" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="6">
         <v>2</v>
       </c>
-      <c r="T25" s="6">
-        <v>1</v>
-      </c>
-      <c r="U25" s="6">
+      <c r="Z25" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="6">
         <v>40</v>
       </c>
-      <c r="V25" s="6">
-        <v>1</v>
-      </c>
-      <c r="W25" s="6">
-        <v>4</v>
-      </c>
-      <c r="X25" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y25" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="6">
+      <c r="AB25" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD25" s="6">
+        <v>4</v>
+      </c>
+      <c r="AE25" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="6">
         <v>5</v>
       </c>
-      <c r="AA25" s="6">
+      <c r="AG25" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="6"/>
     </row>
-    <row r="26" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C26" s="13">
         <v>105004</v>
       </c>
@@ -3866,56 +4320,62 @@
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
-      <c r="M26" s="8">
-        <v>4</v>
-      </c>
-      <c r="N26" s="8">
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8">
+        <v>4</v>
+      </c>
+      <c r="T26" s="8">
         <v>0.2</v>
       </c>
-      <c r="O26" s="8">
+      <c r="U26" s="8">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>5</v>
       </c>
-      <c r="P26" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="8">
+      <c r="V26" s="8">
+        <v>0</v>
+      </c>
+      <c r="W26" s="8">
         <v>20</v>
       </c>
-      <c r="R26" s="8">
-        <v>0</v>
-      </c>
-      <c r="S26" s="8">
+      <c r="X26" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="8">
         <v>1.5</v>
       </c>
-      <c r="T26" s="8">
-        <v>1</v>
-      </c>
-      <c r="U26" s="8">
+      <c r="Z26" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="8">
         <v>20</v>
       </c>
-      <c r="V26" s="8">
-        <v>1</v>
-      </c>
-      <c r="W26" s="8">
-        <v>4</v>
-      </c>
-      <c r="X26" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y26" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="8">
+      <c r="AB26" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD26" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE26" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF26" s="8">
         <v>5</v>
       </c>
-      <c r="AA26" s="8">
+      <c r="AG26" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB26" s="8"/>
-      <c r="AC26" s="8"/>
+      <c r="AH26" s="8"/>
+      <c r="AI26" s="8"/>
     </row>
-    <row r="27" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C27" s="12">
         <v>106001</v>
       </c>
@@ -3930,56 +4390,62 @@
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
-      <c r="M27" s="6">
-        <v>1</v>
-      </c>
-      <c r="N27" s="6">
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6">
+        <v>1</v>
+      </c>
+      <c r="T27" s="6">
         <v>0.5</v>
       </c>
-      <c r="O27" s="6">
+      <c r="U27" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>2</v>
       </c>
-      <c r="P27" s="6">
+      <c r="V27" s="6">
         <v>10</v>
       </c>
-      <c r="Q27" s="6">
-        <v>0</v>
-      </c>
-      <c r="R27" s="6">
-        <v>0</v>
-      </c>
-      <c r="S27" s="6">
-        <v>0</v>
-      </c>
-      <c r="T27" s="6">
-        <v>1</v>
-      </c>
-      <c r="U27" s="6">
+      <c r="W27" s="6">
+        <v>0</v>
+      </c>
+      <c r="X27" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="6">
         <v>12</v>
       </c>
-      <c r="V27" s="6">
-        <v>1</v>
-      </c>
-      <c r="W27" s="6">
-        <v>4</v>
-      </c>
-      <c r="X27" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="6">
+      <c r="AB27" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC27" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD27" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="6"/>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="6"/>
     </row>
-    <row r="28" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C28" s="13">
         <v>106002</v>
       </c>
@@ -3994,56 +4460,62 @@
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
-      <c r="M28" s="8">
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8">
         <v>2</v>
       </c>
-      <c r="N28" s="8">
-        <v>1</v>
-      </c>
-      <c r="O28" s="6">
+      <c r="T28" s="8">
+        <v>1</v>
+      </c>
+      <c r="U28" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>1</v>
       </c>
-      <c r="P28" s="8">
+      <c r="V28" s="8">
         <v>20</v>
       </c>
-      <c r="Q28" s="8">
-        <v>0</v>
-      </c>
-      <c r="R28" s="8">
-        <v>0</v>
-      </c>
-      <c r="S28" s="8">
-        <v>1</v>
-      </c>
-      <c r="T28" s="8">
-        <v>1</v>
-      </c>
-      <c r="U28" s="8">
+      <c r="W28" s="8">
+        <v>0</v>
+      </c>
+      <c r="X28" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="8">
         <v>16</v>
       </c>
-      <c r="V28" s="8">
-        <v>1</v>
-      </c>
-      <c r="W28" s="8">
-        <v>4</v>
-      </c>
-      <c r="X28" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y28" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="8">
+      <c r="AB28" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC28" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD28" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE28" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="8">
         <v>5</v>
       </c>
-      <c r="AA28" s="8">
+      <c r="AG28" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB28" s="8"/>
-      <c r="AC28" s="8"/>
+      <c r="AH28" s="8"/>
+      <c r="AI28" s="8"/>
     </row>
-    <row r="29" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C29" s="12">
         <v>106003</v>
       </c>
@@ -4058,56 +4530,62 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
-      <c r="M29" s="6">
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6">
         <v>3</v>
       </c>
-      <c r="N29" s="6">
+      <c r="T29" s="6">
         <v>2</v>
       </c>
-      <c r="O29" s="6">
+      <c r="U29" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>0.5</v>
       </c>
-      <c r="P29" s="6">
+      <c r="V29" s="6">
         <v>-100</v>
       </c>
-      <c r="Q29" s="6">
-        <v>0</v>
-      </c>
-      <c r="R29" s="6">
-        <v>0</v>
-      </c>
-      <c r="S29" s="6">
+      <c r="W29" s="6">
+        <v>0</v>
+      </c>
+      <c r="X29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="6">
         <v>2</v>
       </c>
-      <c r="T29" s="6">
-        <v>1</v>
-      </c>
-      <c r="U29" s="6">
+      <c r="Z29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="6">
         <v>40</v>
       </c>
-      <c r="V29" s="6">
-        <v>1</v>
-      </c>
-      <c r="W29" s="6">
-        <v>4</v>
-      </c>
-      <c r="X29" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y29" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="6">
+      <c r="AB29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC29" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD29" s="6">
+        <v>4</v>
+      </c>
+      <c r="AE29" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF29" s="6">
         <v>5</v>
       </c>
-      <c r="AA29" s="6">
+      <c r="AG29" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB29" s="6"/>
-      <c r="AC29" s="6"/>
+      <c r="AH29" s="6"/>
+      <c r="AI29" s="6"/>
     </row>
-    <row r="30" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C30" s="13">
         <v>106004</v>
       </c>
@@ -4122,56 +4600,62 @@
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
-      <c r="M30" s="8">
-        <v>4</v>
-      </c>
-      <c r="N30" s="8">
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8">
+        <v>4</v>
+      </c>
+      <c r="T30" s="8">
         <v>0.2</v>
       </c>
-      <c r="O30" s="6">
+      <c r="U30" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>5</v>
       </c>
-      <c r="P30" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="8">
+      <c r="V30" s="8">
+        <v>0</v>
+      </c>
+      <c r="W30" s="8">
         <v>20</v>
       </c>
-      <c r="R30" s="8">
-        <v>0</v>
-      </c>
-      <c r="S30" s="8">
+      <c r="X30" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="8">
         <v>1.5</v>
       </c>
-      <c r="T30" s="8">
-        <v>1</v>
-      </c>
-      <c r="U30" s="8">
+      <c r="Z30" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="8">
         <v>20</v>
       </c>
-      <c r="V30" s="8">
-        <v>1</v>
-      </c>
-      <c r="W30" s="8">
-        <v>4</v>
-      </c>
-      <c r="X30" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y30" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z30" s="8">
+      <c r="AB30" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD30" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE30" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF30" s="8">
         <v>5</v>
       </c>
-      <c r="AA30" s="8">
+      <c r="AG30" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB30" s="8"/>
-      <c r="AC30" s="8"/>
+      <c r="AH30" s="8"/>
+      <c r="AI30" s="8"/>
     </row>
-    <row r="31" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C31" s="12">
         <v>107001</v>
       </c>
@@ -4186,56 +4670,62 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
-      <c r="M31" s="6">
-        <v>1</v>
-      </c>
-      <c r="N31" s="6">
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6">
+        <v>1</v>
+      </c>
+      <c r="T31" s="6">
         <v>0.5</v>
       </c>
-      <c r="O31" s="6">
+      <c r="U31" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>2</v>
       </c>
-      <c r="P31" s="6">
+      <c r="V31" s="6">
         <v>10</v>
       </c>
-      <c r="Q31" s="6">
-        <v>0</v>
-      </c>
-      <c r="R31" s="6">
-        <v>0</v>
-      </c>
-      <c r="S31" s="6">
-        <v>0</v>
-      </c>
-      <c r="T31" s="6">
-        <v>1</v>
-      </c>
-      <c r="U31" s="6">
+      <c r="W31" s="6">
+        <v>0</v>
+      </c>
+      <c r="X31" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="6">
         <v>12</v>
       </c>
-      <c r="V31" s="6">
-        <v>1</v>
-      </c>
-      <c r="W31" s="6">
-        <v>4</v>
-      </c>
-      <c r="X31" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA31" s="6">
+      <c r="AB31" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD31" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF31" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB31" s="6"/>
-      <c r="AC31" s="6"/>
+      <c r="AH31" s="6"/>
+      <c r="AI31" s="6"/>
     </row>
-    <row r="32" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C32" s="13">
         <v>107002</v>
       </c>
@@ -4250,56 +4740,62 @@
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="8">
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8">
         <v>2</v>
       </c>
-      <c r="N32" s="8">
-        <v>1</v>
-      </c>
-      <c r="O32" s="6">
+      <c r="T32" s="8">
+        <v>1</v>
+      </c>
+      <c r="U32" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>1</v>
       </c>
-      <c r="P32" s="8">
+      <c r="V32" s="8">
         <v>20</v>
       </c>
-      <c r="Q32" s="8">
-        <v>0</v>
-      </c>
-      <c r="R32" s="8">
-        <v>0</v>
-      </c>
-      <c r="S32" s="8">
-        <v>1</v>
-      </c>
-      <c r="T32" s="8">
-        <v>1</v>
-      </c>
-      <c r="U32" s="8">
+      <c r="W32" s="8">
+        <v>0</v>
+      </c>
+      <c r="X32" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="8">
         <v>16</v>
       </c>
-      <c r="V32" s="8">
-        <v>1</v>
-      </c>
-      <c r="W32" s="8">
-        <v>4</v>
-      </c>
-      <c r="X32" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y32" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="8">
+      <c r="AB32" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD32" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE32" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="8">
         <v>5</v>
       </c>
-      <c r="AA32" s="8">
+      <c r="AG32" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB32" s="8"/>
-      <c r="AC32" s="8"/>
+      <c r="AH32" s="8"/>
+      <c r="AI32" s="8"/>
     </row>
-    <row r="33" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C33" s="12">
         <v>107003</v>
       </c>
@@ -4314,56 +4810,62 @@
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
-      <c r="M33" s="6">
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6">
         <v>3</v>
       </c>
-      <c r="N33" s="6">
+      <c r="T33" s="6">
         <v>2</v>
       </c>
-      <c r="O33" s="6">
+      <c r="U33" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>0.5</v>
       </c>
-      <c r="P33" s="6">
+      <c r="V33" s="6">
         <v>-100</v>
       </c>
-      <c r="Q33" s="6">
-        <v>0</v>
-      </c>
-      <c r="R33" s="6">
-        <v>0</v>
-      </c>
-      <c r="S33" s="6">
+      <c r="W33" s="6">
+        <v>0</v>
+      </c>
+      <c r="X33" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="6">
         <v>2</v>
       </c>
-      <c r="T33" s="6">
-        <v>1</v>
-      </c>
-      <c r="U33" s="6">
+      <c r="Z33" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="6">
         <v>40</v>
       </c>
-      <c r="V33" s="6">
-        <v>1</v>
-      </c>
-      <c r="W33" s="6">
-        <v>4</v>
-      </c>
-      <c r="X33" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y33" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="6">
+      <c r="AB33" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="6">
+        <v>4</v>
+      </c>
+      <c r="AD33" s="6">
+        <v>4</v>
+      </c>
+      <c r="AE33" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="6">
         <v>5</v>
       </c>
-      <c r="AA33" s="6">
+      <c r="AG33" s="6">
         <v>1010011</v>
       </c>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
+      <c r="AH33" s="6"/>
+      <c r="AI33" s="6"/>
     </row>
-    <row r="34" spans="3:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:35" x14ac:dyDescent="0.2">
       <c r="C34" s="13">
         <v>107004</v>
       </c>
@@ -4378,54 +4880,60 @@
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="8">
-        <v>4</v>
-      </c>
-      <c r="N34" s="8">
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8">
+        <v>4</v>
+      </c>
+      <c r="T34" s="8">
         <v>0.2</v>
       </c>
-      <c r="O34" s="6">
+      <c r="U34" s="6">
         <f>1/表5[[#This Row],[ACT条速度]]</f>
         <v>5</v>
       </c>
-      <c r="P34" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="8">
+      <c r="V34" s="8">
+        <v>0</v>
+      </c>
+      <c r="W34" s="8">
         <v>20</v>
       </c>
-      <c r="R34" s="8">
-        <v>0</v>
-      </c>
-      <c r="S34" s="8">
+      <c r="X34" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="8">
         <v>1.5</v>
       </c>
-      <c r="T34" s="8">
-        <v>1</v>
-      </c>
-      <c r="U34" s="8">
+      <c r="Z34" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="8">
         <v>20</v>
       </c>
-      <c r="V34" s="8">
-        <v>1</v>
-      </c>
-      <c r="W34" s="8">
-        <v>4</v>
-      </c>
-      <c r="X34" s="8">
-        <v>4</v>
-      </c>
-      <c r="Y34" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="8">
+      <c r="AB34" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD34" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE34" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="8">
         <v>5</v>
       </c>
-      <c r="AA34" s="8">
+      <c r="AG34" s="8">
         <v>1010011</v>
       </c>
-      <c r="AB34" s="8"/>
-      <c r="AC34" s="8"/>
+      <c r="AH34" s="8"/>
+      <c r="AI34" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:61e316f commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev ...
</commit_message>
<xml_diff>
--- a/config/excel/SkillBase.xlsx
+++ b/config/excel/SkillBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E173D322-D86B-4DC4-9220-E5F7391AD114}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCFF686-757B-45F4-B38E-DD3D39292B8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,13 +270,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1-选定空间
-2-选定自身
-3-友军单体
-4-敌军单体</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>主目标类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -661,11 +654,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1-从自身
-2-从目标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>skillLaunch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -675,6 +663,18 @@
   </si>
   <si>
     <t>int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-自身周围
+1-选定空间
+2-友军单体
+3-敌军单体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-以自身
+2-以目标</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2306,14 +2306,14 @@
     <tableColumn id="12" xr3:uid="{1B5EF81A-42C1-4ABA-9344-C6A99BE25752}" name="次数限制" dataDxfId="10"/>
     <tableColumn id="13" xr3:uid="{56EA1AC2-2D75-4ECA-AD42-6DEB09A89621}" name="出手范围" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{BA72201D-9EED-4B06-A696-7CF31B0A111F}" name="主目标_x000a_范围类型" dataDxfId="8"/>
-    <tableColumn id="35" xr3:uid="{1706F4DD-D7A0-417E-8EC3-C61A57331DC3}" name="技能_x000a_发起类型" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{A1D82393-11AC-4336-BF23-F777E5F410C1}" name="主目标类型" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{029C5084-1ADB-4FF0-9EBA-349BC28A742D}" name="技能范围长" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{EF7800E1-1840-402E-9BB8-20A4F289955F}" name="技能范围宽" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{12954E63-58B7-4619-80B8-FF4A0AD335D8}" name="作用对象_x000a_技能范围内" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{5457B104-DB84-4AFB-86B6-8E837635CACE}" name="技能效果" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{C8756896-E46D-4763-9CAA-7FE80B81D848}" name="引导技能_x000a_跳数" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{0F0F19EC-5984-4308-A14D-39F32E66077B}" name="引导技能_x000a_间隔" dataDxfId="1"/>
+    <tableColumn id="35" xr3:uid="{1706F4DD-D7A0-417E-8EC3-C61A57331DC3}" name="技能_x000a_发起类型" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{A1D82393-11AC-4336-BF23-F777E5F410C1}" name="主目标类型" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{029C5084-1ADB-4FF0-9EBA-349BC28A742D}" name="技能范围长" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{EF7800E1-1840-402E-9BB8-20A4F289955F}" name="技能范围宽" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{12954E63-58B7-4619-80B8-FF4A0AD335D8}" name="作用对象_x000a_技能范围内" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{5457B104-DB84-4AFB-86B6-8E837635CACE}" name="技能效果" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{C8756896-E46D-4763-9CAA-7FE80B81D848}" name="引导技能_x000a_跳数" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{0F0F19EC-5984-4308-A14D-39F32E66077B}" name="引导技能_x000a_间隔" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2584,8 +2584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2596,8 +2596,8 @@
     <col min="13" max="20" width="10.625" style="1"/>
     <col min="21" max="23" width="11.75" style="1" customWidth="1"/>
     <col min="24" max="30" width="10.625" style="1"/>
-    <col min="31" max="33" width="12.125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="12.125" style="1" customWidth="1"/>
+    <col min="33" max="34" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="16384" width="10.625" style="1"/>
   </cols>
@@ -2613,7 +2613,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>5</v>
@@ -2625,37 +2625,37 @@
         <v>15</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J1" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>16</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q1" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S1" s="16" t="s">
         <v>50</v>
@@ -2664,7 +2664,7 @@
         <v>22</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V1" s="15" t="s">
         <v>19</v>
@@ -2682,34 +2682,34 @@
         <v>33</v>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB1" s="15" t="s">
         <v>53</v>
       </c>
       <c r="AC1" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AD1" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE1" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF1" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="AF1" s="15" t="s">
-        <v>130</v>
-      </c>
       <c r="AG1" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AH1" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AI1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ1" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="AJ1" s="18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2717,10 +2717,10 @@
         <v>49</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>51</v>
@@ -2730,89 +2730,89 @@
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="O2" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>52</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AC2" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="AG2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI2" s="19" t="s">
+      <c r="AJ2" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="AJ2" s="19" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
@@ -2823,7 +2823,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>8</v>
@@ -2835,35 +2835,35 @@
         <v>14</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="O3" s="7"/>
       <c r="P3" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S3" s="7" t="s">
         <v>30</v>
@@ -2894,7 +2894,7 @@
         <v>40</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AD3" s="7" t="s">
         <v>41</v>
@@ -2909,7 +2909,7 @@
         <v>39</v>
       </c>
       <c r="AH3" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
@@ -2922,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>6</v>
@@ -2934,41 +2934,41 @@
         <v>13</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="R4" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U4" s="7"/>
       <c r="V4" s="7" t="s">
@@ -2993,7 +2993,7 @@
         <v>29</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AD4" s="7" t="s">
         <v>44</v>
@@ -3008,14 +3008,14 @@
         <v>47</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -3072,19 +3072,19 @@
         <v>23</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>23</v>
@@ -3094,59 +3094,59 @@
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U6" s="7"/>
       <c r="V6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AB6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AD6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AG6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="AH6" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
@@ -3207,7 +3207,7 @@
         <v>1</v>
       </c>
       <c r="AD7" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE7" s="6">
         <v>2</v>
@@ -3280,7 +3280,7 @@
         <v>2</v>
       </c>
       <c r="AD8" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE8" s="8">
         <v>4</v>
@@ -3353,7 +3353,7 @@
         <v>2</v>
       </c>
       <c r="AD9" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE9" s="6">
         <v>4</v>
@@ -3426,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="AD10" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE10" s="8">
         <v>4</v>
@@ -3499,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="AD11" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE11" s="6">
         <v>4</v>
@@ -3572,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="AD12" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE12" s="8">
         <v>4</v>
@@ -3645,7 +3645,7 @@
         <v>2</v>
       </c>
       <c r="AD13" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE13" s="6">
         <v>4</v>
@@ -3718,7 +3718,7 @@
         <v>2</v>
       </c>
       <c r="AD14" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE14" s="8">
         <v>4</v>
@@ -3791,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="AD15" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE15" s="6">
         <v>2</v>
@@ -3864,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="AD16" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE16" s="8">
         <v>4</v>
@@ -3937,7 +3937,7 @@
         <v>2</v>
       </c>
       <c r="AD17" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE17" s="6">
         <v>4</v>
@@ -4010,7 +4010,7 @@
         <v>2</v>
       </c>
       <c r="AD18" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE18" s="8">
         <v>4</v>
@@ -4083,7 +4083,7 @@
         <v>1</v>
       </c>
       <c r="AD19" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE19" s="6">
         <v>2</v>
@@ -4156,7 +4156,7 @@
         <v>2</v>
       </c>
       <c r="AD20" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE20" s="8">
         <v>4</v>
@@ -4229,7 +4229,7 @@
         <v>2</v>
       </c>
       <c r="AD21" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE21" s="6">
         <v>4</v>
@@ -4302,7 +4302,7 @@
         <v>2</v>
       </c>
       <c r="AD22" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE22" s="8">
         <v>4</v>
@@ -4375,7 +4375,7 @@
         <v>1</v>
       </c>
       <c r="AD23" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE23" s="6">
         <v>2</v>
@@ -4448,7 +4448,7 @@
         <v>2</v>
       </c>
       <c r="AD24" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE24" s="8">
         <v>4</v>
@@ -4521,7 +4521,7 @@
         <v>2</v>
       </c>
       <c r="AD25" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE25" s="6">
         <v>4</v>
@@ -4594,7 +4594,7 @@
         <v>2</v>
       </c>
       <c r="AD26" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE26" s="8">
         <v>4</v>
@@ -4667,7 +4667,7 @@
         <v>1</v>
       </c>
       <c r="AD27" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE27" s="6">
         <v>2</v>
@@ -4740,7 +4740,7 @@
         <v>2</v>
       </c>
       <c r="AD28" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE28" s="8">
         <v>4</v>
@@ -4813,7 +4813,7 @@
         <v>2</v>
       </c>
       <c r="AD29" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE29" s="6">
         <v>4</v>
@@ -4886,7 +4886,7 @@
         <v>2</v>
       </c>
       <c r="AD30" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE30" s="8">
         <v>4</v>
@@ -4959,7 +4959,7 @@
         <v>1</v>
       </c>
       <c r="AD31" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE31" s="6">
         <v>2</v>
@@ -5032,7 +5032,7 @@
         <v>2</v>
       </c>
       <c r="AD32" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE32" s="8">
         <v>4</v>
@@ -5105,7 +5105,7 @@
         <v>2</v>
       </c>
       <c r="AD33" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE33" s="6">
         <v>4</v>
@@ -5178,7 +5178,7 @@
         <v>2</v>
       </c>
       <c r="AD34" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE34" s="8">
         <v>4</v>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:777d0e4 commit_msg:表头顺序调整 ...
</commit_message>
<xml_diff>
--- a/config/excel/SkillBase.xlsx
+++ b/config/excel/SkillBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCFF686-757B-45F4-B38E-DD3D39292B8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2028FC4-3A37-4D1C-8033-A0589910380E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillBase" sheetId="1" r:id="rId1"/>
@@ -2306,14 +2306,14 @@
     <tableColumn id="12" xr3:uid="{1B5EF81A-42C1-4ABA-9344-C6A99BE25752}" name="次数限制" dataDxfId="10"/>
     <tableColumn id="13" xr3:uid="{56EA1AC2-2D75-4ECA-AD42-6DEB09A89621}" name="出手范围" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{BA72201D-9EED-4B06-A696-7CF31B0A111F}" name="主目标_x000a_范围类型" dataDxfId="8"/>
-    <tableColumn id="35" xr3:uid="{1706F4DD-D7A0-417E-8EC3-C61A57331DC3}" name="技能_x000a_发起类型" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{A1D82393-11AC-4336-BF23-F777E5F410C1}" name="主目标类型" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{029C5084-1ADB-4FF0-9EBA-349BC28A742D}" name="技能范围长" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{EF7800E1-1840-402E-9BB8-20A4F289955F}" name="技能范围宽" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{12954E63-58B7-4619-80B8-FF4A0AD335D8}" name="作用对象_x000a_技能范围内" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{5457B104-DB84-4AFB-86B6-8E837635CACE}" name="技能效果" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{C8756896-E46D-4763-9CAA-7FE80B81D848}" name="引导技能_x000a_跳数" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{0F0F19EC-5984-4308-A14D-39F32E66077B}" name="引导技能_x000a_间隔" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{A1D82393-11AC-4336-BF23-F777E5F410C1}" name="主目标类型" dataDxfId="0"/>
+    <tableColumn id="35" xr3:uid="{1706F4DD-D7A0-417E-8EC3-C61A57331DC3}" name="技能_x000a_发起类型" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{029C5084-1ADB-4FF0-9EBA-349BC28A742D}" name="技能范围长" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{EF7800E1-1840-402E-9BB8-20A4F289955F}" name="技能范围宽" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{12954E63-58B7-4619-80B8-FF4A0AD335D8}" name="作用对象_x000a_技能范围内" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{5457B104-DB84-4AFB-86B6-8E837635CACE}" name="技能效果" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{C8756896-E46D-4763-9CAA-7FE80B81D848}" name="引导技能_x000a_跳数" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{0F0F19EC-5984-4308-A14D-39F32E66077B}" name="引导技能_x000a_间隔" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2584,8 +2584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2595,11 +2595,11 @@
     <col min="12" max="12" width="15.625" style="1" customWidth="1"/>
     <col min="13" max="20" width="10.625" style="1"/>
     <col min="21" max="23" width="11.75" style="1" customWidth="1"/>
-    <col min="24" max="30" width="10.625" style="1"/>
-    <col min="31" max="32" width="12.125" style="1" customWidth="1"/>
-    <col min="33" max="34" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="10.625" style="1"/>
+    <col min="24" max="31" width="10.625" style="1"/>
+    <col min="32" max="33" width="12.125" style="1" customWidth="1"/>
+    <col min="34" max="35" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
@@ -2688,10 +2688,10 @@
         <v>53</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="AE1" s="15" t="s">
         <v>128</v>
@@ -2791,10 +2791,10 @@
         <v>90</v>
       </c>
       <c r="AC2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="AE2" s="5" t="s">
         <v>89</v>
@@ -2894,10 +2894,10 @@
         <v>40</v>
       </c>
       <c r="AC3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD3" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="AE3" s="7" t="s">
         <v>42</v>
@@ -2993,10 +2993,10 @@
         <v>29</v>
       </c>
       <c r="AC4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD4" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="AD4" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="AE4" s="7" t="s">
         <v>45</v>
@@ -3131,10 +3131,10 @@
         <v>9</v>
       </c>
       <c r="AC6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>9</v>
       </c>
       <c r="AE6" s="7" t="s">
         <v>96</v>
@@ -3204,10 +3204,10 @@
         <v>1</v>
       </c>
       <c r="AC7" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="6">
         <v>3</v>
+      </c>
+      <c r="AD7" s="21">
+        <v>1</v>
       </c>
       <c r="AE7" s="6">
         <v>2</v>
@@ -3277,10 +3277,10 @@
         <v>1</v>
       </c>
       <c r="AC8" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD8" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE8" s="8">
         <v>4</v>
@@ -3350,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="AC9" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD9" s="6">
         <v>3</v>
+      </c>
+      <c r="AD9" s="21">
+        <v>2</v>
       </c>
       <c r="AE9" s="6">
         <v>4</v>
@@ -3423,10 +3423,10 @@
         <v>1</v>
       </c>
       <c r="AC10" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD10" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE10" s="8">
         <v>4</v>
@@ -3496,10 +3496,10 @@
         <v>1</v>
       </c>
       <c r="AC11" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="6">
         <v>3</v>
+      </c>
+      <c r="AD11" s="21">
+        <v>1</v>
       </c>
       <c r="AE11" s="6">
         <v>4</v>
@@ -3569,10 +3569,10 @@
         <v>1</v>
       </c>
       <c r="AC12" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD12" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE12" s="8">
         <v>4</v>
@@ -3642,10 +3642,10 @@
         <v>1</v>
       </c>
       <c r="AC13" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD13" s="6">
         <v>3</v>
+      </c>
+      <c r="AD13" s="21">
+        <v>2</v>
       </c>
       <c r="AE13" s="6">
         <v>4</v>
@@ -3715,10 +3715,10 @@
         <v>1</v>
       </c>
       <c r="AC14" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD14" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE14" s="8">
         <v>4</v>
@@ -3788,10 +3788,10 @@
         <v>1</v>
       </c>
       <c r="AC15" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD15" s="6">
         <v>3</v>
+      </c>
+      <c r="AD15" s="21">
+        <v>1</v>
       </c>
       <c r="AE15" s="6">
         <v>2</v>
@@ -3861,10 +3861,10 @@
         <v>1</v>
       </c>
       <c r="AC16" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD16" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE16" s="8">
         <v>4</v>
@@ -3934,10 +3934,10 @@
         <v>1</v>
       </c>
       <c r="AC17" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD17" s="6">
         <v>3</v>
+      </c>
+      <c r="AD17" s="21">
+        <v>2</v>
       </c>
       <c r="AE17" s="6">
         <v>4</v>
@@ -4007,10 +4007,10 @@
         <v>1</v>
       </c>
       <c r="AC18" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD18" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE18" s="8">
         <v>4</v>
@@ -4080,10 +4080,10 @@
         <v>1</v>
       </c>
       <c r="AC19" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="6">
         <v>3</v>
+      </c>
+      <c r="AD19" s="21">
+        <v>1</v>
       </c>
       <c r="AE19" s="6">
         <v>2</v>
@@ -4153,10 +4153,10 @@
         <v>1</v>
       </c>
       <c r="AC20" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD20" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE20" s="8">
         <v>4</v>
@@ -4226,10 +4226,10 @@
         <v>1</v>
       </c>
       <c r="AC21" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD21" s="6">
         <v>3</v>
+      </c>
+      <c r="AD21" s="21">
+        <v>2</v>
       </c>
       <c r="AE21" s="6">
         <v>4</v>
@@ -4299,10 +4299,10 @@
         <v>1</v>
       </c>
       <c r="AC22" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD22" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE22" s="8">
         <v>4</v>
@@ -4372,10 +4372,10 @@
         <v>1</v>
       </c>
       <c r="AC23" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD23" s="6">
         <v>3</v>
+      </c>
+      <c r="AD23" s="21">
+        <v>1</v>
       </c>
       <c r="AE23" s="6">
         <v>2</v>
@@ -4445,10 +4445,10 @@
         <v>1</v>
       </c>
       <c r="AC24" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD24" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE24" s="8">
         <v>4</v>
@@ -4518,10 +4518,10 @@
         <v>1</v>
       </c>
       <c r="AC25" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD25" s="6">
         <v>3</v>
+      </c>
+      <c r="AD25" s="21">
+        <v>2</v>
       </c>
       <c r="AE25" s="6">
         <v>4</v>
@@ -4591,10 +4591,10 @@
         <v>1</v>
       </c>
       <c r="AC26" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD26" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE26" s="8">
         <v>4</v>
@@ -4664,10 +4664,10 @@
         <v>1</v>
       </c>
       <c r="AC27" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD27" s="6">
         <v>3</v>
+      </c>
+      <c r="AD27" s="21">
+        <v>1</v>
       </c>
       <c r="AE27" s="6">
         <v>2</v>
@@ -4737,10 +4737,10 @@
         <v>1</v>
       </c>
       <c r="AC28" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD28" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE28" s="8">
         <v>4</v>
@@ -4810,10 +4810,10 @@
         <v>1</v>
       </c>
       <c r="AC29" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD29" s="6">
         <v>3</v>
+      </c>
+      <c r="AD29" s="21">
+        <v>2</v>
       </c>
       <c r="AE29" s="6">
         <v>4</v>
@@ -4883,10 +4883,10 @@
         <v>1</v>
       </c>
       <c r="AC30" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD30" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE30" s="8">
         <v>4</v>
@@ -4956,10 +4956,10 @@
         <v>1</v>
       </c>
       <c r="AC31" s="21">
-        <v>1</v>
-      </c>
-      <c r="AD31" s="6">
         <v>3</v>
+      </c>
+      <c r="AD31" s="21">
+        <v>1</v>
       </c>
       <c r="AE31" s="6">
         <v>2</v>
@@ -5029,10 +5029,10 @@
         <v>1</v>
       </c>
       <c r="AC32" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD32" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE32" s="8">
         <v>4</v>
@@ -5102,10 +5102,10 @@
         <v>1</v>
       </c>
       <c r="AC33" s="21">
-        <v>2</v>
-      </c>
-      <c r="AD33" s="6">
         <v>3</v>
+      </c>
+      <c r="AD33" s="21">
+        <v>2</v>
       </c>
       <c r="AE33" s="6">
         <v>4</v>
@@ -5175,10 +5175,10 @@
         <v>1</v>
       </c>
       <c r="AC34" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD34" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE34" s="8">
         <v>4</v>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:ce34bcf commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev
# Conflicts:
#	global/Att.xlsx ...
</commit_message>
<xml_diff>
--- a/config/excel/SkillBase.xlsx
+++ b/config/excel/SkillBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2028FC4-3A37-4D1C-8033-A0589910380E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCFF686-757B-45F4-B38E-DD3D39292B8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillBase" sheetId="1" r:id="rId1"/>
@@ -2306,14 +2306,14 @@
     <tableColumn id="12" xr3:uid="{1B5EF81A-42C1-4ABA-9344-C6A99BE25752}" name="次数限制" dataDxfId="10"/>
     <tableColumn id="13" xr3:uid="{56EA1AC2-2D75-4ECA-AD42-6DEB09A89621}" name="出手范围" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{BA72201D-9EED-4B06-A696-7CF31B0A111F}" name="主目标_x000a_范围类型" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{A1D82393-11AC-4336-BF23-F777E5F410C1}" name="主目标类型" dataDxfId="0"/>
-    <tableColumn id="35" xr3:uid="{1706F4DD-D7A0-417E-8EC3-C61A57331DC3}" name="技能_x000a_发起类型" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{029C5084-1ADB-4FF0-9EBA-349BC28A742D}" name="技能范围长" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{EF7800E1-1840-402E-9BB8-20A4F289955F}" name="技能范围宽" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{12954E63-58B7-4619-80B8-FF4A0AD335D8}" name="作用对象_x000a_技能范围内" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{5457B104-DB84-4AFB-86B6-8E837635CACE}" name="技能效果" dataDxfId="4"/>
-    <tableColumn id="23" xr3:uid="{C8756896-E46D-4763-9CAA-7FE80B81D848}" name="引导技能_x000a_跳数" dataDxfId="3"/>
-    <tableColumn id="24" xr3:uid="{0F0F19EC-5984-4308-A14D-39F32E66077B}" name="引导技能_x000a_间隔" dataDxfId="2"/>
+    <tableColumn id="35" xr3:uid="{1706F4DD-D7A0-417E-8EC3-C61A57331DC3}" name="技能_x000a_发起类型" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{A1D82393-11AC-4336-BF23-F777E5F410C1}" name="主目标类型" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{029C5084-1ADB-4FF0-9EBA-349BC28A742D}" name="技能范围长" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{EF7800E1-1840-402E-9BB8-20A4F289955F}" name="技能范围宽" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{12954E63-58B7-4619-80B8-FF4A0AD335D8}" name="作用对象_x000a_技能范围内" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{5457B104-DB84-4AFB-86B6-8E837635CACE}" name="技能效果" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{C8756896-E46D-4763-9CAA-7FE80B81D848}" name="引导技能_x000a_跳数" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{0F0F19EC-5984-4308-A14D-39F32E66077B}" name="引导技能_x000a_间隔" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2584,8 +2584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2595,11 +2595,11 @@
     <col min="12" max="12" width="15.625" style="1" customWidth="1"/>
     <col min="13" max="20" width="10.625" style="1"/>
     <col min="21" max="23" width="11.75" style="1" customWidth="1"/>
-    <col min="24" max="31" width="10.625" style="1"/>
-    <col min="32" max="33" width="12.125" style="1" customWidth="1"/>
-    <col min="34" max="35" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="10.625" style="1"/>
+    <col min="24" max="30" width="10.625" style="1"/>
+    <col min="31" max="32" width="12.125" style="1" customWidth="1"/>
+    <col min="33" max="34" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
@@ -2688,10 +2688,10 @@
         <v>53</v>
       </c>
       <c r="AC1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD1" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>130</v>
       </c>
       <c r="AE1" s="15" t="s">
         <v>128</v>
@@ -2791,10 +2791,10 @@
         <v>90</v>
       </c>
       <c r="AC2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="AE2" s="5" t="s">
         <v>89</v>
@@ -2894,10 +2894,10 @@
         <v>40</v>
       </c>
       <c r="AC3" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD3" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="AE3" s="7" t="s">
         <v>42</v>
@@ -2993,10 +2993,10 @@
         <v>29</v>
       </c>
       <c r="AC4" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD4" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="AD4" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="AE4" s="7" t="s">
         <v>45</v>
@@ -3131,10 +3131,10 @@
         <v>9</v>
       </c>
       <c r="AC6" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD6" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="AE6" s="7" t="s">
         <v>96</v>
@@ -3204,10 +3204,10 @@
         <v>1</v>
       </c>
       <c r="AC7" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="6">
         <v>3</v>
-      </c>
-      <c r="AD7" s="21">
-        <v>1</v>
       </c>
       <c r="AE7" s="6">
         <v>2</v>
@@ -3277,10 +3277,10 @@
         <v>1</v>
       </c>
       <c r="AC8" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="8">
         <v>3</v>
-      </c>
-      <c r="AD8" s="8">
-        <v>2</v>
       </c>
       <c r="AE8" s="8">
         <v>4</v>
@@ -3350,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="AC9" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="6">
         <v>3</v>
-      </c>
-      <c r="AD9" s="21">
-        <v>2</v>
       </c>
       <c r="AE9" s="6">
         <v>4</v>
@@ -3423,10 +3423,10 @@
         <v>1</v>
       </c>
       <c r="AC10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="8">
         <v>3</v>
-      </c>
-      <c r="AD10" s="8">
-        <v>2</v>
       </c>
       <c r="AE10" s="8">
         <v>4</v>
@@ -3496,10 +3496,10 @@
         <v>1</v>
       </c>
       <c r="AC11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="6">
         <v>3</v>
-      </c>
-      <c r="AD11" s="21">
-        <v>1</v>
       </c>
       <c r="AE11" s="6">
         <v>4</v>
@@ -3569,10 +3569,10 @@
         <v>1</v>
       </c>
       <c r="AC12" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="8">
         <v>3</v>
-      </c>
-      <c r="AD12" s="8">
-        <v>2</v>
       </c>
       <c r="AE12" s="8">
         <v>4</v>
@@ -3642,10 +3642,10 @@
         <v>1</v>
       </c>
       <c r="AC13" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="6">
         <v>3</v>
-      </c>
-      <c r="AD13" s="21">
-        <v>2</v>
       </c>
       <c r="AE13" s="6">
         <v>4</v>
@@ -3715,10 +3715,10 @@
         <v>1</v>
       </c>
       <c r="AC14" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="8">
         <v>3</v>
-      </c>
-      <c r="AD14" s="8">
-        <v>2</v>
       </c>
       <c r="AE14" s="8">
         <v>4</v>
@@ -3788,10 +3788,10 @@
         <v>1</v>
       </c>
       <c r="AC15" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="6">
         <v>3</v>
-      </c>
-      <c r="AD15" s="21">
-        <v>1</v>
       </c>
       <c r="AE15" s="6">
         <v>2</v>
@@ -3861,10 +3861,10 @@
         <v>1</v>
       </c>
       <c r="AC16" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="8">
         <v>3</v>
-      </c>
-      <c r="AD16" s="8">
-        <v>2</v>
       </c>
       <c r="AE16" s="8">
         <v>4</v>
@@ -3934,10 +3934,10 @@
         <v>1</v>
       </c>
       <c r="AC17" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD17" s="6">
         <v>3</v>
-      </c>
-      <c r="AD17" s="21">
-        <v>2</v>
       </c>
       <c r="AE17" s="6">
         <v>4</v>
@@ -4007,10 +4007,10 @@
         <v>1</v>
       </c>
       <c r="AC18" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD18" s="8">
         <v>3</v>
-      </c>
-      <c r="AD18" s="8">
-        <v>2</v>
       </c>
       <c r="AE18" s="8">
         <v>4</v>
@@ -4080,10 +4080,10 @@
         <v>1</v>
       </c>
       <c r="AC19" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="6">
         <v>3</v>
-      </c>
-      <c r="AD19" s="21">
-        <v>1</v>
       </c>
       <c r="AE19" s="6">
         <v>2</v>
@@ -4153,10 +4153,10 @@
         <v>1</v>
       </c>
       <c r="AC20" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD20" s="8">
         <v>3</v>
-      </c>
-      <c r="AD20" s="8">
-        <v>2</v>
       </c>
       <c r="AE20" s="8">
         <v>4</v>
@@ -4226,10 +4226,10 @@
         <v>1</v>
       </c>
       <c r="AC21" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="6">
         <v>3</v>
-      </c>
-      <c r="AD21" s="21">
-        <v>2</v>
       </c>
       <c r="AE21" s="6">
         <v>4</v>
@@ -4299,10 +4299,10 @@
         <v>1</v>
       </c>
       <c r="AC22" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD22" s="8">
         <v>3</v>
-      </c>
-      <c r="AD22" s="8">
-        <v>2</v>
       </c>
       <c r="AE22" s="8">
         <v>4</v>
@@ -4372,10 +4372,10 @@
         <v>1</v>
       </c>
       <c r="AC23" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="6">
         <v>3</v>
-      </c>
-      <c r="AD23" s="21">
-        <v>1</v>
       </c>
       <c r="AE23" s="6">
         <v>2</v>
@@ -4445,10 +4445,10 @@
         <v>1</v>
       </c>
       <c r="AC24" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD24" s="8">
         <v>3</v>
-      </c>
-      <c r="AD24" s="8">
-        <v>2</v>
       </c>
       <c r="AE24" s="8">
         <v>4</v>
@@ -4518,10 +4518,10 @@
         <v>1</v>
       </c>
       <c r="AC25" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD25" s="6">
         <v>3</v>
-      </c>
-      <c r="AD25" s="21">
-        <v>2</v>
       </c>
       <c r="AE25" s="6">
         <v>4</v>
@@ -4591,10 +4591,10 @@
         <v>1</v>
       </c>
       <c r="AC26" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD26" s="8">
         <v>3</v>
-      </c>
-      <c r="AD26" s="8">
-        <v>2</v>
       </c>
       <c r="AE26" s="8">
         <v>4</v>
@@ -4664,10 +4664,10 @@
         <v>1</v>
       </c>
       <c r="AC27" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="6">
         <v>3</v>
-      </c>
-      <c r="AD27" s="21">
-        <v>1</v>
       </c>
       <c r="AE27" s="6">
         <v>2</v>
@@ -4737,10 +4737,10 @@
         <v>1</v>
       </c>
       <c r="AC28" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="8">
         <v>3</v>
-      </c>
-      <c r="AD28" s="8">
-        <v>2</v>
       </c>
       <c r="AE28" s="8">
         <v>4</v>
@@ -4810,10 +4810,10 @@
         <v>1</v>
       </c>
       <c r="AC29" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD29" s="6">
         <v>3</v>
-      </c>
-      <c r="AD29" s="21">
-        <v>2</v>
       </c>
       <c r="AE29" s="6">
         <v>4</v>
@@ -4883,10 +4883,10 @@
         <v>1</v>
       </c>
       <c r="AC30" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD30" s="8">
         <v>3</v>
-      </c>
-      <c r="AD30" s="8">
-        <v>2</v>
       </c>
       <c r="AE30" s="8">
         <v>4</v>
@@ -4956,10 +4956,10 @@
         <v>1</v>
       </c>
       <c r="AC31" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="6">
         <v>3</v>
-      </c>
-      <c r="AD31" s="21">
-        <v>1</v>
       </c>
       <c r="AE31" s="6">
         <v>2</v>
@@ -5029,10 +5029,10 @@
         <v>1</v>
       </c>
       <c r="AC32" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD32" s="8">
         <v>3</v>
-      </c>
-      <c r="AD32" s="8">
-        <v>2</v>
       </c>
       <c r="AE32" s="8">
         <v>4</v>
@@ -5102,10 +5102,10 @@
         <v>1</v>
       </c>
       <c r="AC33" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD33" s="6">
         <v>3</v>
-      </c>
-      <c r="AD33" s="21">
-        <v>2</v>
       </c>
       <c r="AE33" s="6">
         <v>4</v>
@@ -5175,10 +5175,10 @@
         <v>1</v>
       </c>
       <c r="AC34" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD34" s="8">
         <v>3</v>
-      </c>
-      <c r="AD34" s="8">
-        <v>2</v>
       </c>
       <c r="AE34" s="8">
         <v>4</v>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:64d0038 commit_msg:模型命中点和受击动作配置 ...
</commit_message>
<xml_diff>
--- a/config/excel/SkillBase.xlsx
+++ b/config/excel/SkillBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0F2E65-C0C0-46DB-9283-BECF2D652783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53EFF22-00F7-4D53-90B9-AB3FEEE0C031}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillBase" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="152">
   <si>
     <t>行列头两行不会被读取</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -711,6 +711,34 @@
     <t>距离目标多远使用技能
 近战&lt;目标长
 0-表示不限距离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.767,1.333</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8,1.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8667,1.333,1.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bk1,bk2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bk1,bk3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bk1,bk4,bk5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bk1,bk3,bk5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -895,7 +923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -958,6 +986,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2658,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3263,8 +3294,12 @@
       <c r="K7" s="6">
         <v>2.3330000000000002</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="L7" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
@@ -3343,8 +3378,12 @@
       <c r="K8" s="8">
         <v>2.8330000000000002</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="L8" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
@@ -3423,8 +3462,12 @@
       <c r="K9" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="L9" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -3503,8 +3546,12 @@
       <c r="K10" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+      <c r="L10" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
@@ -3583,8 +3630,12 @@
       <c r="K11" s="6">
         <v>2.3330000000000002</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="L11" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -3663,8 +3714,12 @@
       <c r="K12" s="8">
         <v>2.8330000000000002</v>
       </c>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="L12" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -3743,8 +3798,12 @@
       <c r="K13" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="L13" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
@@ -3823,8 +3882,12 @@
       <c r="K14" s="8">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="L14" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
@@ -3903,8 +3966,12 @@
       <c r="K15" s="6">
         <v>2.3330000000000002</v>
       </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="L15" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
@@ -3983,8 +4050,12 @@
       <c r="K16" s="8">
         <v>2.8330000000000002</v>
       </c>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="L16" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
@@ -4063,8 +4134,12 @@
       <c r="K17" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="L17" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -4143,8 +4218,12 @@
       <c r="K18" s="8">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="L18" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -4223,8 +4302,12 @@
       <c r="K19" s="6">
         <v>2.3330000000000002</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
+      <c r="L19" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
@@ -4303,8 +4386,12 @@
       <c r="K20" s="8">
         <v>2.8330000000000002</v>
       </c>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
+      <c r="L20" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
@@ -4383,8 +4470,12 @@
       <c r="K21" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="L21" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
@@ -4463,8 +4554,12 @@
       <c r="K22" s="8">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="L22" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
@@ -4543,8 +4638,12 @@
       <c r="K23" s="6">
         <v>2.3330000000000002</v>
       </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
+      <c r="L23" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -4623,8 +4722,12 @@
       <c r="K24" s="8">
         <v>2.8330000000000002</v>
       </c>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
+      <c r="L24" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
@@ -4703,8 +4806,12 @@
       <c r="K25" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
@@ -4783,8 +4890,12 @@
       <c r="K26" s="8">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
+      <c r="L26" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
@@ -4863,8 +4974,12 @@
       <c r="K27" s="6">
         <v>2.3330000000000002</v>
       </c>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="L27" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -4943,8 +5058,12 @@
       <c r="K28" s="8">
         <v>2.8330000000000002</v>
       </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="L28" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
@@ -5023,8 +5142,12 @@
       <c r="K29" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="L29" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -5103,8 +5226,12 @@
       <c r="K30" s="8">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="L30" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
@@ -5183,8 +5310,12 @@
       <c r="K31" s="6">
         <v>2.3330000000000002</v>
       </c>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="L31" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
@@ -5263,8 +5394,12 @@
       <c r="K32" s="8">
         <v>2.8330000000000002</v>
       </c>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
+      <c r="L32" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
@@ -5343,8 +5478,12 @@
       <c r="K33" s="6">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
+      <c r="L33" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
@@ -5423,8 +5562,12 @@
       <c r="K34" s="8">
         <v>7.3330000000000002</v>
       </c>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
+      <c r="L34" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>

</xml_diff>